<commit_message>
perf: :zap: Mejoras en rendimiento, funcionalidades agregadas y errores corregidos
Mejoras en rendimiento, funcionalidades agregadas y errores corregidos
</commit_message>
<xml_diff>
--- a/apps/server/src/storage/StudentReview.xlsx
+++ b/apps/server/src/storage/StudentReview.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,63 +479,60 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="str">
         <v>P</v>
       </c>
       <c r="C2" t="str">
-        <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Fusce quis felis hendrerit sapien vestibulum egestas vitae et mi. Sed ac odio ipsum. Phasellus non ultricies ante. Phasellus fermentum ipsum id nulla vehicula, a laoreet urna porta.</v>
+        <v>Prueba de previa en punto de tesis</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>45234.6574537037</v>
+        <v>45310.01892361111</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J2" t="str">
-        <v>Juan</v>
+        <v>Laura Sofía</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L2" t="str">
-        <v>Un nuevo tema más descriptivo</v>
+        <v>Lo bueno de ser bueno</v>
       </c>
       <c r="M2" t="str">
         <v>201020831/preview.pdf</v>
       </c>
-      <c r="N2" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
       <c r="O2" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
       <c r="P2" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="Q2" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="R2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="S2" t="str">
         <v>Marco Antonio</v>
       </c>
       <c r="T2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="str">
         <v>A</v>
@@ -550,51 +547,48 @@
         <v>201020831/dictamen_punto_tesis.pdf</v>
       </c>
       <c r="F3" s="1">
-        <v>45234.71923611111</v>
+        <v>45310.02232638889</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J3" t="str">
-        <v>Juan</v>
+        <v>Laura Sofía</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L3" t="str">
-        <v>Un nuevo tema más descriptivo</v>
+        <v>Lo bueno de ser bueno</v>
       </c>
       <c r="M3" t="str">
         <v>201020831/preview.pdf</v>
       </c>
-      <c r="N3" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
       <c r="O3" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
       <c r="P3" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="Q3" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="R3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="S3" t="str">
         <v>Marco Antonio</v>
       </c>
       <c r="T3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="str">
         <v>A</v>
@@ -609,523 +603,101 @@
         <v>201020831/dictmen_curso_I.pdf</v>
       </c>
       <c r="F4" s="1">
-        <v>45234.75958333333</v>
+        <v>45310.028344907405</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H4" t="str">
         <v>201020831/Nombramiento.pdf</v>
       </c>
       <c r="J4" t="str">
-        <v>Luis</v>
+        <v>Carlos Miguel</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L4" t="str">
-        <v>Un nuevo tema más descriptivo</v>
+        <v>Lo bueno de ser bueno</v>
       </c>
       <c r="M4" t="str">
         <v>201020831/preview.pdf</v>
       </c>
-      <c r="N4" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
       <c r="O4" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
       <c r="P4" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="Q4" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="R4">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="S4" t="str">
         <v>Marco Antonio</v>
       </c>
       <c r="T4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V4" s="1">
-        <v>45235.9999537037</v>
+        <v>45305.9999537037</v>
       </c>
       <c r="W4" t="str">
-        <v>meet.google.com/hnb-wsir-lhk</v>
+        <v>meet.google.com/eps-lorx-fet</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" t="str">
-        <v>A</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Curso aprobado</v>
+        <v>E</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" t="str">
-        <v>201020831/dictamen_curso_II.pdf</v>
-      </c>
       <c r="F5" s="1">
-        <v>45234.771469907406</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Laura</v>
+        <v>45310.028344907405</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L5" t="str">
-        <v>Un nuevo tema más descriptivo</v>
+        <v>Lo bueno de ser bueno</v>
       </c>
       <c r="M5" t="str">
         <v>201020831/preview.pdf</v>
       </c>
-      <c r="N5" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
       <c r="O5" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
       <c r="P5" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="Q5" s="1">
-        <v>45234.587233796294</v>
+        <v>45310.00951388889</v>
       </c>
       <c r="R5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="S5" t="str">
         <v>Marco Antonio</v>
       </c>
       <c r="T5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <v>3</v>
-      </c>
-      <c r="V5" s="1">
-        <v>45242.9999537037</v>
-      </c>
-      <c r="W5" t="str">
-        <v>meet.google.com/hnb-wsir-lhk</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" t="str">
-        <v>P</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Revisión del titulo 2.2 en pag. 6 y del titulo 2.3.4 en pag.15</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45234.790625</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Carlos</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M6" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N6" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O6" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P6" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R6">
-        <v>13</v>
-      </c>
-      <c r="S6" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T6">
-        <v>5</v>
-      </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="str">
-        <v>A</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Se cambió el título de la tesis de: Un tema único y descriptivo a: Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" t="str">
-        <v>201020831/dictamen.pdf</v>
-      </c>
-      <c r="F7" s="1">
-        <v>45234.78702546296</v>
-      </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M7" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N7" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O7" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P7" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R7">
-        <v>13</v>
-      </c>
-      <c r="S7" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T7">
-        <v>5</v>
-      </c>
-      <c r="U7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8" t="str">
-        <v>A</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Documento aprobado</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8" t="str">
-        <v>201020831/dictamen_tesis.pdf</v>
-      </c>
-      <c r="F8" s="1">
-        <v>45234.79115740741</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="J8" t="str">
-        <v>Carlos</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M8" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N8" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O8" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P8" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R8">
-        <v>13</v>
-      </c>
-      <c r="S8" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T8">
-        <v>5</v>
-      </c>
-      <c r="U8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9" t="str">
-        <v>P</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Presentarse con su tesis impresa</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
-        <v>45234.80185185185</v>
-      </c>
-      <c r="G9">
-        <v>11</v>
-      </c>
-      <c r="I9" t="str">
-        <v>310</v>
-      </c>
-      <c r="J9" t="str">
-        <v>Guilmar</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M9" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N9" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O9" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P9" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R9">
-        <v>13</v>
-      </c>
-      <c r="S9" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-      <c r="U9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>13</v>
-      </c>
-      <c r="B10" t="str">
-        <v>A</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Presentar su tesis impresa</v>
-      </c>
-      <c r="D10">
-        <v>6</v>
-      </c>
-      <c r="E10" t="str">
-        <v>201020831/dictamen_prev_internos.pdf</v>
-      </c>
-      <c r="F10" s="1">
-        <v>45234.97574074074</v>
-      </c>
-      <c r="G10">
-        <v>11</v>
-      </c>
-      <c r="I10" t="str">
-        <v>305</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Guilmar</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M10" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N10" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O10" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P10" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R10">
-        <v>13</v>
-      </c>
-      <c r="S10" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T10">
-        <v>5</v>
-      </c>
-      <c r="U10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>19</v>
-      </c>
-      <c r="B11" t="str">
-        <v>A</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Gestión de impresión de tesis</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-      <c r="E11" t="str">
-        <v>201020831/dictamen_impresion.pdf</v>
-      </c>
-      <c r="F11" s="1">
-        <v>45234.976805555554</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="str">
-        <v>320</v>
-      </c>
-      <c r="J11" t="str">
-        <v>Admin</v>
-      </c>
-      <c r="K11">
-        <v>2</v>
-      </c>
-      <c r="L11" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M11" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N11" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O11" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P11" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R11">
-        <v>13</v>
-      </c>
-      <c r="S11" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T11">
-        <v>5</v>
-      </c>
-      <c r="U11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>20</v>
-      </c>
-      <c r="B12" t="str">
-        <v>A</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1">
-        <v>45234.976805555554</v>
-      </c>
-      <c r="K12">
-        <v>2</v>
-      </c>
-      <c r="L12" t="str">
-        <v>Un nuevo tema más descriptivo</v>
-      </c>
-      <c r="M12" t="str">
-        <v>201020831/preview.pdf</v>
-      </c>
-      <c r="N12" t="str">
-        <v>201020831/thesis.pdf</v>
-      </c>
-      <c r="O12" t="str">
-        <v>201020831/asesor.pdf</v>
-      </c>
-      <c r="P12" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>45234.587233796294</v>
-      </c>
-      <c r="R12">
-        <v>13</v>
-      </c>
-      <c r="S12" t="str">
-        <v>Marco Antonio</v>
-      </c>
-      <c r="T12">
-        <v>5</v>
-      </c>
-      <c r="U12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:X12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: :lock: Add require auth middleware
Add require auth middleware in some endpoints necesaries
</commit_message>
<xml_diff>
--- a/apps/server/src/storage/StudentReview.xlsx
+++ b/apps/server/src/storage/StudentReview.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -508,6 +508,9 @@
       <c r="M2" t="str">
         <v>201020831/preview.pdf</v>
       </c>
+      <c r="N2" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
       <c r="O2" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
@@ -564,6 +567,9 @@
       <c r="M3" t="str">
         <v>201020831/preview.pdf</v>
       </c>
+      <c r="N3" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
       <c r="O3" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
@@ -623,6 +629,9 @@
       <c r="M4" t="str">
         <v>201020831/preview.pdf</v>
       </c>
+      <c r="N4" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
       <c r="O4" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
@@ -656,13 +665,25 @@
         <v>12</v>
       </c>
       <c r="B5" t="str">
-        <v>E</v>
+        <v>A</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Curso aprobado</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
+      <c r="E5" t="str">
+        <v>201020831/dictamen_curso_II.pdf</v>
+      </c>
       <c r="F5" s="1">
-        <v>45310.028344907405</v>
+        <v>45310.05960648148</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Carlos Miguel</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -673,6 +694,9 @@
       <c r="M5" t="str">
         <v>201020831/preview.pdf</v>
       </c>
+      <c r="N5" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
       <c r="O5" t="str">
         <v>201020831/asesor.pdf</v>
       </c>
@@ -692,12 +716,316 @@
         <v>1</v>
       </c>
       <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1">
+        <v>45312.9999537037</v>
+      </c>
+      <c r="W5" t="str">
+        <v>meet.google.com/eps-lorx-fet</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="str">
+        <v>A</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Documento aprobado</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="str">
+        <v>201020831/dictamen_tesis.pdf</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45310.063101851854</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="J6" t="str">
+        <v>María Laura</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" t="str">
+        <v>Lo bueno de ser bueno</v>
+      </c>
+      <c r="M6" t="str">
+        <v>201020831/preview.pdf</v>
+      </c>
+      <c r="N6" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
+      <c r="O6" t="str">
+        <v>201020831/asesor.pdf</v>
+      </c>
+      <c r="P6" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6" t="str">
+        <v>Marco Antonio</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="str">
+        <v>P</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45310.07900462963</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="J7" t="str">
+        <v>María Laura</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" t="str">
+        <v>Lo bueno de ser bueno</v>
+      </c>
+      <c r="M7" t="str">
+        <v>201020831/preview.pdf</v>
+      </c>
+      <c r="N7" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
+      <c r="O7" t="str">
+        <v>201020831/asesor.pdf</v>
+      </c>
+      <c r="P7" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7" t="str">
+        <v>Marco Antonio</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" t="str">
+        <v>A</v>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="str">
+        <v>201020831/dictamen_prev_internos.pdf</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45310.08186342593</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="I8" t="str">
+        <v>303</v>
+      </c>
+      <c r="J8" t="str">
+        <v>María Laura</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Lo bueno de ser bueno</v>
+      </c>
+      <c r="M8" t="str">
+        <v>201020831/preview.pdf</v>
+      </c>
+      <c r="N8" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
+      <c r="O8" t="str">
+        <v>201020831/asesor.pdf</v>
+      </c>
+      <c r="P8" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8" t="str">
+        <v>Marco Antonio</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" t="str">
+        <v>A</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Cita para impresión de tesis</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="str">
+        <v>201020831/dictamen_impresion.pdf</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45310.09809027778</v>
+      </c>
+      <c r="G9">
+        <v>24</v>
+      </c>
+      <c r="I9" t="str">
+        <v>200</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Super</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Lo bueno de ser bueno</v>
+      </c>
+      <c r="M9" t="str">
+        <v>201020831/preview.pdf</v>
+      </c>
+      <c r="N9" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
+      <c r="O9" t="str">
+        <v>201020831/asesor.pdf</v>
+      </c>
+      <c r="P9" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9" t="str">
+        <v>Marco Antonio</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" t="str">
+        <v>A</v>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <v>201020831/dictamen_entrega.pdf</v>
+      </c>
+      <c r="F10" s="1">
+        <v>45310.10863425926</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
+      <c r="I10" t="str">
+        <v>303</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Super</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10" t="str">
+        <v>Lo bueno de ser bueno</v>
+      </c>
+      <c r="M10" t="str">
+        <v>201020831/preview.pdf</v>
+      </c>
+      <c r="N10" t="str">
+        <v>201020831/thesis.pdf</v>
+      </c>
+      <c r="O10" t="str">
+        <v>201020831/asesor.pdf</v>
+      </c>
+      <c r="P10" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>45310.00951388889</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
+      <c r="S10" t="str">
+        <v>Marco Antonio</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:X5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>